<commit_message>
Bug: fix co-modified clone cross_module change lines output
</commit_message>
<xml_diff>
--- a/results/apollo_comodify_dup_results.xlsx
+++ b/results/apollo_comodify_dup_results.xlsx
@@ -507,11 +507,11 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'canbus,drivers': 1, 'common,drivers': 3, 'canbus,drivers,localization': 1, 'canbus,common,control,localization,planning': 3, 'common,control,localization': 3, 'canbus,common,control,localization': 2, 'canbus,control': 4, 'canbus,common,control': 1, 'canbus,control,planning': 1, 'control,localization': 1, 'common,control': 2, 'control,planning': 1, 'control,drivers': 1}</t>
+          <t>{'control,localization': 1, 'canbus,drivers,localization': 1, 'canbus,control': 4, 'common,control': 2, 'canbus,common,control': 1, 'control,drivers': 1, 'canbus,common,control,localization,planning': 3, 'common,control,localization': 3, 'canbus,common,control,localization': 2, 'canbus,control,planning': 1, 'common,drivers': 3, 'control,planning': 1, 'canbus,drivers': 1}</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>24</v>
+        <v>646</v>
       </c>
       <c r="I2" t="n">
         <v>5247</v>
@@ -540,11 +540,11 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'canbus,control': 1, 'canbus,common,localization,planning,prediction': 1, 'common,perception': 3, 'canbus,common,control,dreamview,localization,perception,planning,prediction,routing': 2, 'common,localization,planning,prediction': 1, 'common,control,dreamview,localization,perception,planning,prediction': 2, 'canbus,common,control,dreamview,localization,perception,planning,prediction': 5, 'planning,prediction': 6, 'drivers,planning': 1, 'localization,planning,prediction': 1, 'dreamview,routing': 1, 'common,control,perception,planning': 2, 'control,localization': 2, 'control,localization,planning': 2, 'canbus,control,map,perception,planning,prediction,routing': 1, 'drivers,perception,planning': 2, 'canbus,drivers': 2, 'canbus,control,perception': 1, 'control,perception': 3, 'control,planning': 3, 'drivers,perception': 6, 'control,planning,prediction': 1, 'common,map': 2, 'map,planning': 3, 'map,perception,planning': 1, 'drivers,map,perception,planning': 1, 'map,perception': 3, 'map,prediction': 1, 'dreamview,map': 1, 'common,planning': 1, 'drivers,map,perception': 1, 'common,localization': 1, 'calibration,dreamview,planning': 1, 'canbus,perception': 1}</t>
+          <t>{'canbus,control,perception': 1, 'drivers,perception': 6, 'localization,planning,prediction': 1, 'map,planning': 3, 'common,perception': 3, 'canbus,common,control,dreamview,localization,perception,planning,prediction,routing': 2, 'canbus,common,localization,planning,prediction': 1, 'common,localization,planning,prediction': 1, 'common,control,dreamview,localization,perception,planning,prediction': 2, 'canbus,common,control,dreamview,localization,perception,planning,prediction': 5, 'drivers,map,perception,planning': 1, 'map,prediction': 1, 'canbus,control,map,perception,planning,prediction,routing': 1, 'control,planning': 3, 'drivers,planning': 1, 'planning,prediction': 6, 'control,planning,prediction': 1, 'common,control,perception,planning': 2, 'control,perception': 3, 'control,localization': 2, 'control,localization,planning': 2, 'common,map': 2, 'common,planning': 1, 'common,localization': 1, 'drivers,map,perception': 1, 'canbus,drivers': 2, 'map,perception': 3, 'calibration,dreamview,planning': 1, 'dreamview,map': 1, 'map,perception,planning': 1, 'drivers,perception,planning': 2, 'dreamview,routing': 1, 'canbus,control': 1, 'canbus,perception': 1}</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>66</v>
+        <v>1345</v>
       </c>
       <c r="I3" t="n">
         <v>5285</v>
@@ -573,11 +573,11 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>{'canbus,common,control,drivers,localization,perception,planning,prediction': 1, 'calibration,dreamview,perception': 1, 'perception,planning,prediction': 1, 'common,control,localization,perception,planning,prediction': 3, 'canbus,common,control,dreamview,localization,perception,planning,prediction': 3, 'common,control,dreamview,localization,perception,planning,prediction': 4, 'common,control': 1, 'common,control,perception,planning': 1, 'control,planning': 4, 'perception,planning': 4, 'drivers,localization,map,perception': 3, 'control,localization': 4, 'drivers,perception,planning': 1, 'control,drivers': 2, 'control,dreamview,drivers': 1, 'control,localization,perception': 2, 'control,perception,planning,prediction': 1, 'common,localization,perception,planning,prediction': 2, 'dreamview,map,planning,prediction': 2, 'control,prediction': 1, 'common,control,drivers,planning': 1, 'common,localization,planning,prediction': 1, 'localization,planning,prediction': 2, 'localization,planning': 6, 'dreamview,drivers,localization,map,perception': 1, 'planning,prediction': 2, 'perception,prediction': 2, 'common,map': 1, 'localization,map,perception': 2, 'localization,map': 2, 'drivers,map,perception': 1, 'drivers,map': 1, 'perception,planning,prediction,routing': 1, 'map,perception': 1, 'common,map,perception,planning': 1, 'common,perception': 2, 'common,map,perception': 1, 'drivers,localization,perception': 1, 'common,drivers,planning': 1, 'drivers,routing': 1, 'common,planning': 2, 'drivers,perception': 3, 'canbus,control': 1, 'dreamview,map': 1, 'canbus,perception': 1, 'canbus,drivers': 1, 'localization,perception': 1, 'map,planning': 1}</t>
+          <t>{'control,localization,perception': 2, 'common,planning': 2, 'canbus,common,control,drivers,localization,perception,planning,prediction': 1, 'common,control,localization,perception,planning,prediction': 3, 'canbus,common,control,dreamview,localization,perception,planning,prediction': 3, 'common,control,dreamview,localization,perception,planning,prediction': 4, 'perception,planning,prediction': 1, 'localization,map': 2, 'drivers,localization,map,perception': 3, 'perception,planning,prediction,routing': 1, 'perception,planning': 4, 'map,perception': 1, 'planning,prediction': 2, 'localization,planning,prediction': 2, 'perception,prediction': 2, 'control,perception,planning,prediction': 1, 'calibration,dreamview,perception': 1, 'common,control,perception,planning': 1, 'common,drivers,planning': 1, 'common,control,drivers,planning': 1, 'dreamview,drivers,localization,map,perception': 1, 'control,localization': 4, 'common,localization,perception,planning,prediction': 2, 'common,localization,planning,prediction': 1, 'control,drivers': 2, 'control,dreamview,drivers': 1, 'localization,map,perception': 2, 'drivers,localization,perception': 1, 'dreamview,map,planning,prediction': 2, 'common,control': 1, 'control,planning': 4, 'localization,planning': 6, 'dreamview,map': 1, 'drivers,routing': 1, 'common,perception': 2, 'drivers,map,perception': 1, 'drivers,perception,planning': 1, 'control,prediction': 1, 'common,map': 1, 'common,map,perception': 1, 'common,map,perception,planning': 1, 'drivers,map': 1, 'canbus,control': 1, 'drivers,perception': 3, 'canbus,perception': 1, 'map,planning': 1, 'localization,perception': 1, 'canbus,drivers': 1}</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>84</v>
+        <v>2190</v>
       </c>
       <c r="I4" t="n">
         <v>8536</v>
@@ -606,11 +606,11 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>{'canbus,common,drivers,localization,perception,planning,prediction': 1, 'perception,planning,prediction': 2, 'common,control,localization,perception,planning,prediction': 2, 'canbus,common,control,dreamview,localization,map,perception,planning,prediction': 3, 'common,control,dreamview,localization,perception,planning,prediction': 4, 'common,control,dreamview,localization,map,perception,planning,prediction': 2, 'drivers,localization': 7, 'drivers,localization,map,perception': 6, 'drivers,perception': 2, 'localization,perception': 2, 'control,localization': 1, 'control,localization,planning,prediction': 1, 'map,perception': 3, 'planning,prediction': 8, 'control,localization,perception': 1, 'canbus,perception': 2, 'common,localization,perception,planning,prediction': 2, 'localization,perception,planning,prediction': 1, 'control,localization,perception,planning,prediction': 1, 'control,localization,perception,planning': 1, 'control,map': 1, 'map,prediction': 1, 'map,planning,prediction': 1, 'perception,prediction': 1, 'drivers,localization,perception': 1, 'perception,planning': 4, 'localization,planning,prediction': 1, 'common,map': 3, 'dreamview,map,planning,prediction': 2, 'dreamview,map': 4, 'common,localization': 2, 'perception,planning,prediction,routing': 1, 'canbus,drivers': 1, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction,routing': 1, 'control,planning': 3, 'control,localization,planning': 1, 'map,planning': 1, 'localization,planning': 3, 'control,prediction': 1, 'dreamview,localization': 1}</t>
+          <t>{'perception,prediction': 1, 'canbus,perception': 2, 'drivers,localization,perception': 1, 'canbus,common,drivers,localization,perception,planning,prediction': 1, 'common,control,localization,perception,planning,prediction': 2, 'canbus,common,control,dreamview,localization,map,perception,planning,prediction': 3, 'common,control,dreamview,localization,perception,planning,prediction': 4, 'common,control,dreamview,localization,map,perception,planning,prediction': 2, 'drivers,localization,map,perception': 6, 'control,localization,perception': 1, 'planning,prediction': 8, 'localization,planning,prediction': 1, 'map,planning,prediction': 1, 'perception,planning,prediction': 2, 'control,localization': 1, 'control,localization,planning,prediction': 1, 'common,localization': 2, 'map,perception': 3, 'common,localization,perception,planning,prediction': 2, 'drivers,localization': 7, 'perception,planning': 4, 'drivers,perception': 2, 'dreamview,map': 4, 'dreamview,map,planning,prediction': 2, 'localization,perception,planning,prediction': 1, 'control,localization,perception,planning,prediction': 1, 'control,localization,perception,planning': 1, 'perception,planning,prediction,routing': 1, 'common,map': 3, 'localization,perception': 2, 'map,prediction': 1, 'control,map': 1, 'map,planning': 1, 'control,planning': 3, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction,routing': 1, 'control,localization,planning': 1, 'localization,planning': 3, 'control,prediction': 1, 'canbus,drivers': 1, 'dreamview,localization': 1}</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>86</v>
+        <v>2239</v>
       </c>
       <c r="I5" t="n">
         <v>8590</v>
@@ -639,11 +639,11 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>{'planning,prediction': 6, 'planning,prediction,routing': 1, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction,routing': 1, 'canbus,common,control,dreamview,localization,map,perception,planning,prediction': 1, 'canbus,common,control,dreamview,localization,perception,planning,prediction': 5, 'control,prediction': 2, 'control,localization,planning,prediction': 2, 'drivers,localization': 4, 'control,planning': 3, 'control,localization': 1, 'control,localization,planning': 1, 'control,map': 1, 'dreamview,map,planning,prediction': 2, 'common,control,dreamview,localization,perception,planning,prediction': 7, 'common,dreamview,localization,perception,planning,prediction': 1, 'common,localization,perception,planning,prediction': 2, 'localization,perception,planning,prediction': 1, 'perception,planning,prediction': 3, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction': 1, 'perception,planning': 3, 'drivers,planning': 1, 'dreamview,map': 5, 'localization,planning,prediction': 1, 'perception,prediction': 1, 'drivers,localization,map': 5, 'common,map': 4, 'map,planning': 2, 'localization,planning': 3, 'common,drivers': 2, 'common,perception': 1, 'control,drivers,map': 1, 'control,drivers': 1, 'control,map,prediction': 1, 'common,localization': 1, 'localization,map': 1, 'dreamview,localization': 1}</t>
+          <t>{'planning,prediction': 6, 'map,planning': 2, 'dreamview,map,planning,prediction': 2, 'dreamview,map': 5, 'control,localization': 1, 'drivers,planning': 1, 'control,planning': 3, 'control,localization,planning,prediction': 2, 'localization,planning,prediction': 1, 'perception,planning,prediction': 3, 'control,prediction': 2, 'perception,prediction': 1, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction,routing': 1, 'canbus,common,control,dreamview,localization,map,perception,planning,prediction': 1, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction': 1, 'control,localization,planning': 1, 'drivers,localization': 4, 'drivers,localization,map': 5, 'planning,prediction,routing': 1, 'common,drivers': 2, 'common,perception': 1, 'canbus,common,control,dreamview,localization,perception,planning,prediction': 5, 'common,control,dreamview,localization,perception,planning,prediction': 7, 'common,dreamview,localization,perception,planning,prediction': 1, 'common,localization,perception,planning,prediction': 2, 'control,drivers,map': 1, 'control,drivers': 1, 'perception,planning': 3, 'localization,perception,planning,prediction': 1, 'localization,planning': 3, 'common,map': 4, 'control,map,prediction': 1, 'common,localization': 1, 'control,map': 1, 'dreamview,localization': 1, 'localization,map': 1}</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>79</v>
+        <v>1914</v>
       </c>
       <c r="I6" t="n">
         <v>7057</v>
@@ -672,11 +672,11 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>{'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction': 1, 'drivers,perception': 2, 'perception,planning': 16, 'control,planning': 9, 'control,localization,perception,planning': 1, 'control,perception,planning': 1, 'perception,prediction': 5, 'canbus,common,control,drivers,localization,map,perception,planning,prediction,v2x': 2, 'canbus,common,control,localization,perception,planning,prediction,v2x': 2, 'canbus,common,control,localization,perception,planning,prediction': 2, 'canbus,common,control,dreamview,localization,perception,planning,prediction,v2x': 1, 'drivers,localization,routing': 1, 'common,perception': 5, 'monitor,perception': 1, 'drivers,localization,map,perception,planning': 2, 'control,perception': 4, 'dreamview,map,perception,planning,prediction': 1, 'control,map': 1, 'control,localization,map': 2, 'localization,perception': 3, 'control,localization': 1, 'dreamview,map,perception,prediction': 1, 'common,control,localization,perception,planning,prediction': 1, 'common,control,dreamview,localization,perception,planning,prediction': 2, 'common,localization,perception,planning,prediction': 1, 'common,localization,planning,prediction': 1, 'localization,planning,prediction': 1, 'planning,prediction': 12, 'drivers,prediction': 1, 'common,map': 2, 'localization,map': 2, 'perception,v2x': 2, 'dreamview,localization': 1, 'localization,perception,planning,prediction': 1, 'perception,planning,prediction': 1, 'map,v2x': 1, 'dreamview,map,prediction': 1, 'drivers,planning': 1, 'dreamview,map': 1, 'drivers,localization': 2, 'common,planning': 2, 'map,perception': 3, 'drivers,localization,map,perception': 1, 'localization,planning': 2, 'canbus,control': 2, 'map,planning': 1, 'drivers,map': 2, 'localization,tools': 2, 'map,tools': 1, 'control,drivers': 1, 'dreamview,perception': 2}</t>
+          <t>{'perception,v2x': 2, 'drivers,localization': 2, 'dreamview,localization': 1, 'planning,prediction': 12, 'localization,perception,planning,prediction': 1, 'perception,planning,prediction': 1, 'perception,prediction': 5, 'canbus,common,control,dreamview,drivers,localization,map,perception,planning,prediction': 1, 'drivers,localization,map,perception,planning': 2, 'drivers,localization,map,perception': 1, 'control,planning': 9, 'perception,planning': 16, 'control,localization,perception,planning': 1, 'control,perception,planning': 1, 'monitor,perception': 1, 'canbus,common,control,drivers,localization,map,perception,planning,prediction,v2x': 2, 'map,planning': 1, 'common,map': 2, 'canbus,common,control,localization,perception,planning,prediction,v2x': 2, 'common,perception': 5, 'canbus,common,control,localization,perception,planning,prediction': 2, 'canbus,common,control,dreamview,localization,perception,planning,prediction,v2x': 1, 'common,control,localization,perception,planning,prediction': 1, 'common,control,dreamview,localization,perception,planning,prediction': 2, 'common,localization,perception,planning,prediction': 1, 'common,localization,planning,prediction': 1, 'map,v2x': 1, 'drivers,planning': 1, 'drivers,perception': 2, 'localization,planning,prediction': 1, 'drivers,map': 2, 'dreamview,map,perception,planning,prediction': 1, 'dreamview,map,perception,prediction': 1, 'dreamview,map,prediction': 1, 'dreamview,map': 1, 'control,localization,map': 2, 'localization,planning': 2, 'localization,map': 2, 'common,planning': 2, 'control,map': 1, 'control,perception': 4, 'control,localization': 1, 'map,perception': 3, 'drivers,localization,routing': 1, 'canbus,control': 2, 'drivers,prediction': 1, 'localization,perception': 3, 'localization,tools': 2, 'control,drivers': 1, 'map,tools': 1, 'dreamview,perception': 2}</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>117</v>
+        <v>1642</v>
       </c>
       <c r="I7" t="n">
         <v>12108</v>
@@ -705,11 +705,11 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>{'canbus,common,control,data,dreamview,drivers,localization,map,perception,planning,prediction': 1, 'localization,planning': 1, 'common,control,localization,perception,planning,prediction': 2, 'common,control,dreamview,localization,perception,planning,prediction': 5, 'canbus,common,control,dreamview,localization,perception,planning,prediction,v2x': 2, 'canbus,drivers': 3, 'control,planning': 6, 'control,drivers,perception,planning': 1, 'drivers,perception': 1, 'localization,perception': 6, 'perception,planning': 10, 'common,localization,perception,planning,prediction': 1, 'common,localization,planning,prediction': 1, 'common,planning,prediction': 1, 'planning,prediction': 9, 'map,perception': 7, 'canbus,common,control,drivers,localization,map,perception,planning,v2x': 1, 'canbus,common,control,drivers,localization,perception,planning,v2x': 1, 'canbus,common,control,localization,perception,planning,v2x': 3, 'common,perception': 1, 'control,perception': 4, 'control,perception,planning': 4, 'map,planning': 3, 'canbus,common,control,localization,perception,planning': 1, 'common,prediction': 4, 'drivers,planning': 3, 'control,localization,perception,planning,prediction': 1, 'dreamview,map,perception,planning': 1, 'guardian,monitor': 1, 'dreamview,prediction': 1, 'localization,tools': 2, 'localization,map': 1, 'dreamview,map': 3, 'map,tools': 1, 'dreamview,planning': 1, 'drivers,localization,map,perception': 1, 'localization,map,perception': 2, 'dreamview,map,perception': 1, 'dreamview,perception': 1, 'drivers,map': 1, 'map,v2x': 1, 'drivers,localization': 2, 'map,prediction': 1, 'common,planning': 1}</t>
+          <t>{'canbus,common,control,data,dreamview,drivers,localization,map,perception,planning,prediction': 1, 'common,prediction': 4, 'control,perception': 4, 'control,perception,planning': 4, 'perception,planning': 10, 'guardian,monitor': 1, 'dreamview,prediction': 1, 'common,control,dreamview,localization,perception,planning,prediction': 5, 'canbus,common,control,dreamview,localization,perception,planning,prediction,v2x': 2, 'planning,prediction': 9, 'localization,planning': 1, 'drivers,planning': 3, 'control,localization,perception,planning,prediction': 1, 'localization,tools': 2, 'map,tools': 1, 'localization,perception': 6, 'control,drivers,perception,planning': 1, 'control,planning': 6, 'canbus,common,control,localization,perception,planning': 1, 'common,control,localization,perception,planning,prediction': 2, 'common,localization,perception,planning,prediction': 1, 'common,localization,planning,prediction': 1, 'common,planning,prediction': 1, 'common,perception': 1, 'map,perception': 7, 'canbus,drivers': 3, 'canbus,common,control,drivers,localization,map,perception,planning,v2x': 1, 'map,planning': 3, 'canbus,common,control,drivers,localization,perception,planning,v2x': 1, 'canbus,common,control,localization,perception,planning,v2x': 3, 'localization,map': 1, 'dreamview,map,perception,planning': 1, 'dreamview,map': 3, 'drivers,perception': 1, 'map,v2x': 1, 'dreamview,map,perception': 1, 'localization,map,perception': 2, 'drivers,localization,map,perception': 1, 'drivers,localization': 2, 'dreamview,planning': 1, 'dreamview,perception': 1, 'drivers,map': 1, 'map,prediction': 1, 'common,planning': 1}</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>105</v>
+        <v>1696</v>
       </c>
       <c r="I8" t="n">
         <v>15696</v>

</xml_diff>